<commit_message>
java memory problems and solving them
</commit_message>
<xml_diff>
--- a/Definitions/b_Definitions_Tools.xlsx
+++ b/Definitions/b_Definitions_Tools.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="755" uniqueCount="655">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="757" uniqueCount="657">
   <si>
     <t>Topics</t>
   </si>
@@ -3305,6 +3305,12 @@
   </si>
   <si>
     <t>git add /path/file1.txt</t>
+  </si>
+  <si>
+    <t>push the changes to git repository without entering credentials</t>
+  </si>
+  <si>
+    <t>git push origin --all</t>
   </si>
 </sst>
 </file>
@@ -3521,7 +3527,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="80">
+  <cellXfs count="82">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -3663,6 +3669,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3670,12 +3677,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3710,6 +3717,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -4086,10 +4094,10 @@
       </c>
     </row>
     <row r="13" spans="1:3">
-      <c r="A13" s="63" t="s">
+      <c r="A13" s="64" t="s">
         <v>255</v>
       </c>
-      <c r="B13" s="64"/>
+      <c r="B13" s="65"/>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" s="1" t="s">
@@ -4135,10 +4143,10 @@
       </c>
     </row>
     <row r="23" spans="1:2">
-      <c r="A23" s="63" t="s">
+      <c r="A23" s="64" t="s">
         <v>331</v>
       </c>
-      <c r="B23" s="64"/>
+      <c r="B23" s="65"/>
     </row>
     <row r="24" spans="1:2">
       <c r="A24" s="1" t="s">
@@ -4151,10 +4159,10 @@
       </c>
     </row>
     <row r="27" spans="1:2">
-      <c r="A27" s="63" t="s">
+      <c r="A27" s="64" t="s">
         <v>616</v>
       </c>
-      <c r="B27" s="64"/>
+      <c r="B27" s="65"/>
     </row>
     <row r="28" spans="1:2">
       <c r="A28" s="1" t="s">
@@ -4220,10 +4228,10 @@
     </row>
     <row r="3" spans="1:2" s="17" customFormat="1"/>
     <row r="11" spans="1:2">
-      <c r="A11" s="63" t="s">
+      <c r="A11" s="64" t="s">
         <v>3</v>
       </c>
-      <c r="B11" s="64"/>
+      <c r="B11" s="65"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -4261,10 +4269,10 @@
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="63" t="s">
+      <c r="A2" s="64" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="64"/>
+      <c r="B2" s="65"/>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="58" t="s">
@@ -4331,7 +4339,7 @@
       </c>
     </row>
     <row r="11" spans="1:2">
-      <c r="A11" s="76" t="s">
+      <c r="A11" s="77" t="s">
         <v>635</v>
       </c>
       <c r="B11" s="59" t="s">
@@ -4339,7 +4347,7 @@
       </c>
     </row>
     <row r="12" spans="1:2">
-      <c r="A12" s="76"/>
+      <c r="A12" s="77"/>
       <c r="B12" s="59" t="s">
         <v>637</v>
       </c>
@@ -4409,10 +4417,10 @@
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="63" t="s">
+      <c r="A2" s="64" t="s">
         <v>254</v>
       </c>
-      <c r="B2" s="64"/>
+      <c r="B2" s="65"/>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="50" t="s">
@@ -4423,10 +4431,10 @@
       </c>
     </row>
     <row r="6" spans="1:2">
-      <c r="A6" s="63" t="s">
+      <c r="A6" s="64" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="64"/>
+      <c r="B6" s="65"/>
     </row>
     <row r="7" spans="1:2" ht="30">
       <c r="A7" s="49" t="s">
@@ -4559,7 +4567,7 @@
       </c>
     </row>
     <row r="24" spans="1:2" ht="45">
-      <c r="A24" s="69" t="s">
+      <c r="A24" s="70" t="s">
         <v>545</v>
       </c>
       <c r="B24" s="48" t="s">
@@ -4567,13 +4575,13 @@
       </c>
     </row>
     <row r="25" spans="1:2" ht="90">
-      <c r="A25" s="69"/>
+      <c r="A25" s="70"/>
       <c r="B25" s="48" t="s">
         <v>547</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="30">
-      <c r="A26" s="69"/>
+      <c r="A26" s="70"/>
       <c r="B26" s="48" t="s">
         <v>548</v>
       </c>
@@ -4599,7 +4607,7 @@
       </c>
     </row>
     <row r="30" spans="1:2" ht="60">
-      <c r="A30" s="78" t="s">
+      <c r="A30" s="79" t="s">
         <v>553</v>
       </c>
       <c r="B30" s="48" t="s">
@@ -4607,25 +4615,25 @@
       </c>
     </row>
     <row r="31" spans="1:2" ht="180">
-      <c r="A31" s="78"/>
+      <c r="A31" s="79"/>
       <c r="B31" s="48" t="s">
         <v>554</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="60">
-      <c r="A32" s="78"/>
+      <c r="A32" s="79"/>
       <c r="B32" s="48" t="s">
         <v>556</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="45">
-      <c r="A33" s="78"/>
+      <c r="A33" s="79"/>
       <c r="B33" s="48" t="s">
         <v>557</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="45">
-      <c r="A34" s="78" t="s">
+      <c r="A34" s="79" t="s">
         <v>558</v>
       </c>
       <c r="B34" s="48" t="s">
@@ -4633,19 +4641,19 @@
       </c>
     </row>
     <row r="35" spans="1:2" ht="105">
-      <c r="A35" s="78"/>
+      <c r="A35" s="79"/>
       <c r="B35" s="48" t="s">
         <v>560</v>
       </c>
     </row>
     <row r="36" spans="1:2">
-      <c r="A36" s="78"/>
+      <c r="A36" s="79"/>
       <c r="B36" s="48" t="s">
         <v>561</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="75">
-      <c r="A37" s="78" t="s">
+      <c r="A37" s="79" t="s">
         <v>562</v>
       </c>
       <c r="B37" s="48" t="s">
@@ -4653,25 +4661,25 @@
       </c>
     </row>
     <row r="38" spans="1:2" ht="120">
-      <c r="A38" s="78"/>
+      <c r="A38" s="79"/>
       <c r="B38" s="48" t="s">
         <v>564</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="45">
-      <c r="A39" s="78"/>
+      <c r="A39" s="79"/>
       <c r="B39" s="48" t="s">
         <v>565</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="45">
-      <c r="A40" s="78"/>
+      <c r="A40" s="79"/>
       <c r="B40" s="48" t="s">
         <v>566</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="60">
-      <c r="A41" s="78" t="s">
+      <c r="A41" s="79" t="s">
         <v>567</v>
       </c>
       <c r="B41" s="48" t="s">
@@ -4679,25 +4687,25 @@
       </c>
     </row>
     <row r="42" spans="1:2" ht="105">
-      <c r="A42" s="78"/>
+      <c r="A42" s="79"/>
       <c r="B42" s="48" t="s">
         <v>569</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="45">
-      <c r="A43" s="78"/>
+      <c r="A43" s="79"/>
       <c r="B43" s="48" t="s">
         <v>570</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="135">
-      <c r="A44" s="78"/>
+      <c r="A44" s="79"/>
       <c r="B44" s="48" t="s">
         <v>571</v>
       </c>
     </row>
     <row r="45" spans="1:2">
-      <c r="A45" s="78"/>
+      <c r="A45" s="79"/>
       <c r="B45" s="48" t="s">
         <v>572</v>
       </c>
@@ -4912,10 +4920,10 @@
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="63" t="s">
+      <c r="A2" s="64" t="s">
         <v>254</v>
       </c>
-      <c r="B2" s="64"/>
+      <c r="B2" s="65"/>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="50" t="s">
@@ -4926,10 +4934,10 @@
       </c>
     </row>
     <row r="6" spans="1:2">
-      <c r="A6" s="63" t="s">
+      <c r="A6" s="64" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="64"/>
+      <c r="B6" s="65"/>
     </row>
     <row r="7" spans="1:2" ht="30">
       <c r="A7" s="66" t="s">
@@ -4986,7 +4994,7 @@
       </c>
     </row>
     <row r="14" spans="1:2" ht="45">
-      <c r="A14" s="72"/>
+      <c r="A14" s="73"/>
       <c r="B14" s="44" t="s">
         <v>505</v>
       </c>
@@ -5032,7 +5040,7 @@
       </c>
     </row>
     <row r="20" spans="1:2" ht="75">
-      <c r="A20" s="72" t="s">
+      <c r="A20" s="73" t="s">
         <v>517</v>
       </c>
       <c r="B20" s="48" t="s">
@@ -5040,13 +5048,13 @@
       </c>
     </row>
     <row r="21" spans="1:2" ht="75">
-      <c r="A21" s="72"/>
+      <c r="A21" s="73"/>
       <c r="B21" s="48" t="s">
         <v>519</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="30">
-      <c r="A22" s="79" t="s">
+      <c r="A22" s="80" t="s">
         <v>300</v>
       </c>
       <c r="B22" s="48" t="s">
@@ -5054,13 +5062,13 @@
       </c>
     </row>
     <row r="23" spans="1:2" ht="150">
-      <c r="A23" s="79"/>
+      <c r="A23" s="80"/>
       <c r="B23" s="48" t="s">
         <v>521</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="45">
-      <c r="A24" s="79" t="s">
+      <c r="A24" s="80" t="s">
         <v>454</v>
       </c>
       <c r="B24" s="48" t="s">
@@ -5068,13 +5076,13 @@
       </c>
     </row>
     <row r="25" spans="1:2" ht="150">
-      <c r="A25" s="79"/>
+      <c r="A25" s="80"/>
       <c r="B25" s="48" t="s">
         <v>523</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="60">
-      <c r="A26" s="72" t="s">
+      <c r="A26" s="73" t="s">
         <v>524</v>
       </c>
       <c r="B26" s="48" t="s">
@@ -5082,25 +5090,25 @@
       </c>
     </row>
     <row r="27" spans="1:2" ht="30">
-      <c r="A27" s="72"/>
+      <c r="A27" s="73"/>
       <c r="B27" s="48" t="s">
         <v>526</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="30">
-      <c r="A28" s="72"/>
+      <c r="A28" s="73"/>
       <c r="B28" s="48" t="s">
         <v>527</v>
       </c>
     </row>
     <row r="29" spans="1:2">
-      <c r="A29" s="72"/>
+      <c r="A29" s="73"/>
       <c r="B29" s="48" t="s">
         <v>528</v>
       </c>
     </row>
     <row r="30" spans="1:2">
-      <c r="A30" s="72" t="s">
+      <c r="A30" s="73" t="s">
         <v>531</v>
       </c>
       <c r="B30" s="48" t="s">
@@ -5108,7 +5116,7 @@
       </c>
     </row>
     <row r="31" spans="1:2" ht="30">
-      <c r="A31" s="72"/>
+      <c r="A31" s="73"/>
       <c r="B31" s="48" t="s">
         <v>530</v>
       </c>
@@ -5157,16 +5165,16 @@
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="63" t="s">
+      <c r="A2" s="64" t="s">
         <v>254</v>
       </c>
-      <c r="B2" s="64"/>
+      <c r="B2" s="65"/>
     </row>
     <row r="6" spans="1:2">
-      <c r="A6" s="63" t="s">
+      <c r="A6" s="64" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="64"/>
+      <c r="B6" s="65"/>
     </row>
     <row r="7" spans="1:2" ht="30">
       <c r="A7" s="22" t="s">
@@ -5222,10 +5230,10 @@
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="63" t="s">
+      <c r="A2" s="64" t="s">
         <v>254</v>
       </c>
-      <c r="B2" s="64"/>
+      <c r="B2" s="65"/>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="52" t="s">
@@ -5236,10 +5244,10 @@
       </c>
     </row>
     <row r="6" spans="1:2">
-      <c r="A6" s="63" t="s">
+      <c r="A6" s="64" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="64"/>
+      <c r="B6" s="65"/>
     </row>
     <row r="7" spans="1:2" ht="75">
       <c r="A7" s="53" t="s">
@@ -5303,16 +5311,16 @@
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="63" t="s">
+      <c r="A2" s="64" t="s">
         <v>254</v>
       </c>
-      <c r="B2" s="64"/>
+      <c r="B2" s="65"/>
     </row>
     <row r="6" spans="1:2">
-      <c r="A6" s="63" t="s">
+      <c r="A6" s="64" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="64"/>
+      <c r="B6" s="65"/>
     </row>
     <row r="7" spans="1:2" ht="45">
       <c r="A7" s="22" t="s">
@@ -5368,10 +5376,10 @@
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="63" t="s">
+      <c r="A2" s="64" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="64"/>
+      <c r="B2" s="65"/>
     </row>
     <row r="3" spans="1:2" ht="60">
       <c r="A3" s="30" t="s">
@@ -5682,10 +5690,10 @@
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="63" t="s">
+      <c r="A2" s="64" t="s">
         <v>228</v>
       </c>
-      <c r="B2" s="64"/>
+      <c r="B2" s="65"/>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="21" t="s">
@@ -5704,10 +5712,10 @@
       </c>
     </row>
     <row r="7" spans="1:2">
-      <c r="A7" s="63" t="s">
+      <c r="A7" s="64" t="s">
         <v>229</v>
       </c>
-      <c r="B7" s="64"/>
+      <c r="B7" s="65"/>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="6" t="s">
@@ -5724,10 +5732,10 @@
       <c r="A10" s="6"/>
     </row>
     <row r="11" spans="1:2">
-      <c r="A11" s="63" t="s">
+      <c r="A11" s="64" t="s">
         <v>103</v>
       </c>
-      <c r="B11" s="64"/>
+      <c r="B11" s="65"/>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="19" t="s">
@@ -5770,10 +5778,10 @@
       </c>
     </row>
     <row r="17" spans="1:2">
-      <c r="A17" s="63" t="s">
+      <c r="A17" s="64" t="s">
         <v>329</v>
       </c>
-      <c r="B17" s="64"/>
+      <c r="B17" s="65"/>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="31" t="s">
@@ -5784,10 +5792,10 @@
       </c>
     </row>
     <row r="20" spans="1:2">
-      <c r="A20" s="63" t="s">
+      <c r="A20" s="64" t="s">
         <v>436</v>
       </c>
-      <c r="B20" s="64"/>
+      <c r="B20" s="65"/>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" s="31" t="s">
@@ -5798,10 +5806,10 @@
       </c>
     </row>
     <row r="23" spans="1:2">
-      <c r="A23" s="63" t="s">
+      <c r="A23" s="64" t="s">
         <v>209</v>
       </c>
-      <c r="B23" s="64"/>
+      <c r="B23" s="65"/>
     </row>
     <row r="24" spans="1:2">
       <c r="A24" s="17" t="s">
@@ -5828,10 +5836,10 @@
       </c>
     </row>
     <row r="28" spans="1:2">
-      <c r="A28" s="63" t="s">
+      <c r="A28" s="64" t="s">
         <v>205</v>
       </c>
-      <c r="B28" s="64"/>
+      <c r="B28" s="65"/>
     </row>
     <row r="29" spans="1:2">
       <c r="A29" s="17" t="s">
@@ -5850,10 +5858,10 @@
       </c>
     </row>
     <row r="32" spans="1:2">
-      <c r="A32" s="63" t="s">
+      <c r="A32" s="64" t="s">
         <v>104</v>
       </c>
-      <c r="B32" s="64"/>
+      <c r="B32" s="65"/>
     </row>
     <row r="33" spans="1:2">
       <c r="A33" s="19" t="s">
@@ -5872,10 +5880,10 @@
       </c>
     </row>
     <row r="36" spans="1:2">
-      <c r="A36" s="63" t="s">
+      <c r="A36" s="64" t="s">
         <v>168</v>
       </c>
-      <c r="B36" s="64"/>
+      <c r="B36" s="65"/>
     </row>
     <row r="37" spans="1:2">
       <c r="A37" s="19" t="s">
@@ -5886,10 +5894,10 @@
       </c>
     </row>
     <row r="39" spans="1:2">
-      <c r="A39" s="63" t="s">
+      <c r="A39" s="64" t="s">
         <v>171</v>
       </c>
-      <c r="B39" s="64"/>
+      <c r="B39" s="65"/>
     </row>
     <row r="40" spans="1:2">
       <c r="A40" t="s">
@@ -5906,16 +5914,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A17:B17"/>
     <mergeCell ref="A23:B23"/>
     <mergeCell ref="A28:B28"/>
     <mergeCell ref="A32:B32"/>
     <mergeCell ref="A36:B36"/>
     <mergeCell ref="A39:B39"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A17:B17"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B1" location="Materials!A2" display="Up"/>
@@ -5963,10 +5971,10 @@
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="63" t="s">
+      <c r="A2" s="64" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="64"/>
+      <c r="B2" s="65"/>
     </row>
     <row r="3" spans="1:2" ht="45">
       <c r="A3" s="30" t="s">
@@ -6009,7 +6017,7 @@
       </c>
     </row>
     <row r="8" spans="1:2" ht="94.5">
-      <c r="A8" s="65" t="s">
+      <c r="A8" s="68" t="s">
         <v>409</v>
       </c>
       <c r="B8" s="35" t="s">
@@ -6017,7 +6025,7 @@
       </c>
     </row>
     <row r="9" spans="1:2" ht="126">
-      <c r="A9" s="65"/>
+      <c r="A9" s="68"/>
       <c r="B9" s="35" t="s">
         <v>411</v>
       </c>
@@ -6133,11 +6141,11 @@
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
+      <selection pane="bottomLeft" activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6155,10 +6163,10 @@
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="63" t="s">
+      <c r="A2" s="64" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="64"/>
+      <c r="B2" s="65"/>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="56" t="s">
@@ -6225,7 +6233,7 @@
       </c>
     </row>
     <row r="11" spans="1:2">
-      <c r="A11" s="76" t="s">
+      <c r="A11" s="77" t="s">
         <v>650</v>
       </c>
       <c r="B11" s="61" t="s">
@@ -6233,9 +6241,17 @@
       </c>
     </row>
     <row r="12" spans="1:2">
-      <c r="A12" s="76"/>
+      <c r="A12" s="77"/>
       <c r="B12" s="61" t="s">
         <v>652</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" s="81" t="s">
+        <v>655</v>
+      </c>
+      <c r="B13" s="63" t="s">
+        <v>656</v>
       </c>
     </row>
   </sheetData>
@@ -6275,10 +6291,10 @@
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="63" t="s">
+      <c r="A2" s="64" t="s">
         <v>254</v>
       </c>
-      <c r="B2" s="64"/>
+      <c r="B2" s="65"/>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="24" t="s">
@@ -6289,10 +6305,10 @@
       </c>
     </row>
     <row r="10" spans="1:2">
-      <c r="A10" s="63" t="s">
+      <c r="A10" s="64" t="s">
         <v>3</v>
       </c>
-      <c r="B10" s="64"/>
+      <c r="B10" s="65"/>
     </row>
     <row r="11" spans="1:2" ht="45">
       <c r="A11" s="6" t="s">
@@ -6383,7 +6399,7 @@
       </c>
     </row>
     <row r="22" spans="1:2">
-      <c r="A22" s="65" t="s">
+      <c r="A22" s="68" t="s">
         <v>26</v>
       </c>
       <c r="B22" s="6" t="s">
@@ -6391,13 +6407,13 @@
       </c>
     </row>
     <row r="23" spans="1:2">
-      <c r="A23" s="65"/>
+      <c r="A23" s="68"/>
       <c r="B23" s="6" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="24" spans="1:2">
-      <c r="A24" s="69" t="s">
+      <c r="A24" s="70" t="s">
         <v>29</v>
       </c>
       <c r="B24" s="6" t="s">
@@ -6405,7 +6421,7 @@
       </c>
     </row>
     <row r="25" spans="1:2">
-      <c r="A25" s="69"/>
+      <c r="A25" s="70"/>
       <c r="B25" s="6" t="s">
         <v>31</v>
       </c>
@@ -6451,7 +6467,7 @@
       </c>
     </row>
     <row r="31" spans="1:2" ht="45">
-      <c r="A31" s="68" t="s">
+      <c r="A31" s="69" t="s">
         <v>42</v>
       </c>
       <c r="B31" s="51" t="s">
@@ -6459,7 +6475,7 @@
       </c>
     </row>
     <row r="32" spans="1:2" ht="120">
-      <c r="A32" s="68"/>
+      <c r="A32" s="69"/>
       <c r="B32" s="51" t="s">
         <v>43</v>
       </c>
@@ -6647,7 +6663,7 @@
       </c>
     </row>
     <row r="57" spans="1:2" ht="60">
-      <c r="A57" s="65" t="s">
+      <c r="A57" s="68" t="s">
         <v>87</v>
       </c>
       <c r="B57" s="6" t="s">
@@ -6655,19 +6671,19 @@
       </c>
     </row>
     <row r="58" spans="1:2" ht="45">
-      <c r="A58" s="65"/>
+      <c r="A58" s="68"/>
       <c r="B58" s="6" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="59" spans="1:2" ht="60">
-      <c r="A59" s="65"/>
+      <c r="A59" s="68"/>
       <c r="B59" s="6" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="60" spans="1:2" ht="30">
-      <c r="A60" s="65"/>
+      <c r="A60" s="68"/>
       <c r="B60" s="6" t="s">
         <v>91</v>
       </c>
@@ -6681,7 +6697,7 @@
       </c>
     </row>
     <row r="62" spans="1:2" ht="30">
-      <c r="A62" s="65" t="s">
+      <c r="A62" s="68" t="s">
         <v>94</v>
       </c>
       <c r="B62" s="6" t="s">
@@ -6689,7 +6705,7 @@
       </c>
     </row>
     <row r="63" spans="1:2">
-      <c r="A63" s="65"/>
+      <c r="A63" s="68"/>
       <c r="B63" s="6" t="s">
         <v>102</v>
       </c>
@@ -6859,7 +6875,7 @@
       </c>
     </row>
     <row r="85" spans="1:2" ht="30">
-      <c r="A85" s="65" t="s">
+      <c r="A85" s="68" t="s">
         <v>288</v>
       </c>
       <c r="B85" s="25" t="s">
@@ -6867,7 +6883,7 @@
       </c>
     </row>
     <row r="86" spans="1:2" ht="90">
-      <c r="A86" s="65"/>
+      <c r="A86" s="68"/>
       <c r="B86" s="25" t="s">
         <v>290</v>
       </c>
@@ -6973,7 +6989,7 @@
       </c>
     </row>
     <row r="100" spans="1:2" ht="30">
-      <c r="A100" s="65" t="s">
+      <c r="A100" s="68" t="s">
         <v>316</v>
       </c>
       <c r="B100" s="28" t="s">
@@ -6981,7 +6997,7 @@
       </c>
     </row>
     <row r="101" spans="1:2">
-      <c r="A101" s="65"/>
+      <c r="A101" s="68"/>
       <c r="B101" s="28" t="s">
         <v>318</v>
       </c>
@@ -7150,6 +7166,25 @@
     </row>
   </sheetData>
   <mergeCells count="26">
+    <mergeCell ref="A100:A101"/>
+    <mergeCell ref="A102:A103"/>
+    <mergeCell ref="A104:A105"/>
+    <mergeCell ref="A106:A107"/>
+    <mergeCell ref="A85:A86"/>
+    <mergeCell ref="A96:A97"/>
+    <mergeCell ref="A98:A99"/>
+    <mergeCell ref="A42:A43"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A31:A32"/>
+    <mergeCell ref="A22:A23"/>
+    <mergeCell ref="A24:A25"/>
+    <mergeCell ref="A68:A69"/>
+    <mergeCell ref="A72:A73"/>
+    <mergeCell ref="A48:A50"/>
+    <mergeCell ref="A51:A53"/>
+    <mergeCell ref="A57:A60"/>
+    <mergeCell ref="A62:A63"/>
     <mergeCell ref="A120:A122"/>
     <mergeCell ref="A123:A124"/>
     <mergeCell ref="A108:A109"/>
@@ -7157,25 +7192,6 @@
     <mergeCell ref="A112:A113"/>
     <mergeCell ref="A114:A115"/>
     <mergeCell ref="A116:A117"/>
-    <mergeCell ref="A68:A69"/>
-    <mergeCell ref="A72:A73"/>
-    <mergeCell ref="A48:A50"/>
-    <mergeCell ref="A51:A53"/>
-    <mergeCell ref="A57:A60"/>
-    <mergeCell ref="A62:A63"/>
-    <mergeCell ref="A42:A43"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A31:A32"/>
-    <mergeCell ref="A22:A23"/>
-    <mergeCell ref="A24:A25"/>
-    <mergeCell ref="A100:A101"/>
-    <mergeCell ref="A102:A103"/>
-    <mergeCell ref="A104:A105"/>
-    <mergeCell ref="A106:A107"/>
-    <mergeCell ref="A85:A86"/>
-    <mergeCell ref="A96:A97"/>
-    <mergeCell ref="A98:A99"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B1" location="JSON!A2" display="Up"/>
@@ -7215,16 +7231,16 @@
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="63" t="s">
+      <c r="A2" s="64" t="s">
         <v>254</v>
       </c>
-      <c r="B2" s="64"/>
+      <c r="B2" s="65"/>
     </row>
     <row r="5" spans="1:2">
-      <c r="A5" s="63" t="s">
+      <c r="A5" s="64" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="64"/>
+      <c r="B5" s="65"/>
     </row>
     <row r="6" spans="1:2" ht="45">
       <c r="A6" t="s">
@@ -7289,10 +7305,10 @@
     </row>
     <row r="3" spans="1:2" s="19" customFormat="1"/>
     <row r="9" spans="1:2">
-      <c r="A9" s="63" t="s">
+      <c r="A9" s="64" t="s">
         <v>3</v>
       </c>
-      <c r="B9" s="64"/>
+      <c r="B9" s="65"/>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
@@ -7347,19 +7363,19 @@
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="63" t="s">
+      <c r="A2" s="64" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="64"/>
+      <c r="B2" s="65"/>
     </row>
     <row r="9" spans="1:2">
-      <c r="A9" s="63" t="s">
+      <c r="A9" s="64" t="s">
         <v>3</v>
       </c>
-      <c r="B9" s="64"/>
+      <c r="B9" s="65"/>
     </row>
     <row r="10" spans="1:2" ht="75">
-      <c r="A10" s="71" t="s">
+      <c r="A10" s="72" t="s">
         <v>112</v>
       </c>
       <c r="B10" s="54" t="s">
@@ -7455,10 +7471,10 @@
       </c>
     </row>
     <row r="23" spans="1:2">
-      <c r="A23" s="70" t="s">
+      <c r="A23" s="71" t="s">
         <v>134</v>
       </c>
-      <c r="B23" s="70"/>
+      <c r="B23" s="71"/>
     </row>
     <row r="24" spans="1:2" ht="60">
       <c r="A24" s="55" t="s">
@@ -7646,16 +7662,16 @@
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="63" t="s">
+      <c r="A2" s="64" t="s">
         <v>254</v>
       </c>
-      <c r="B2" s="64"/>
+      <c r="B2" s="65"/>
     </row>
     <row r="6" spans="1:2">
-      <c r="A6" s="63" t="s">
+      <c r="A6" s="64" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="64"/>
+      <c r="B6" s="65"/>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="43" t="s">
@@ -7666,7 +7682,7 @@
       </c>
     </row>
     <row r="8" spans="1:2" ht="105">
-      <c r="A8" s="72" t="s">
+      <c r="A8" s="73" t="s">
         <v>487</v>
       </c>
       <c r="B8" s="42" t="s">
@@ -7674,7 +7690,7 @@
       </c>
     </row>
     <row r="9" spans="1:2" ht="105">
-      <c r="A9" s="72"/>
+      <c r="A9" s="73"/>
       <c r="B9" s="42" t="s">
         <v>489</v>
       </c>
@@ -7806,20 +7822,20 @@
       </c>
     </row>
     <row r="2" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A2" s="73" t="s">
+      <c r="A2" s="74" t="s">
         <v>172</v>
       </c>
-      <c r="B2" s="74"/>
+      <c r="B2" s="75"/>
     </row>
     <row r="8" spans="1:2" ht="15.75" thickBot="1"/>
     <row r="9" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A9" s="73" t="s">
+      <c r="A9" s="74" t="s">
         <v>3</v>
       </c>
-      <c r="B9" s="74"/>
+      <c r="B9" s="75"/>
     </row>
     <row r="10" spans="1:2">
-      <c r="A10" s="75" t="s">
+      <c r="A10" s="76" t="s">
         <v>185</v>
       </c>
       <c r="B10" t="s">
@@ -7827,13 +7843,13 @@
       </c>
     </row>
     <row r="11" spans="1:2">
-      <c r="A11" s="76"/>
+      <c r="A11" s="77"/>
       <c r="B11" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="12" spans="1:2">
-      <c r="A12" s="77" t="s">
+      <c r="A12" s="78" t="s">
         <v>182</v>
       </c>
       <c r="B12" t="s">
@@ -7841,13 +7857,13 @@
       </c>
     </row>
     <row r="13" spans="1:2" ht="45">
-      <c r="A13" s="77"/>
+      <c r="A13" s="78"/>
       <c r="B13" s="14" t="s">
         <v>180</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="60">
-      <c r="A14" s="77"/>
+      <c r="A14" s="78"/>
       <c r="B14" s="14" t="s">
         <v>179</v>
       </c>

</xml_diff>

<commit_message>
git commands, AWS preperation
</commit_message>
<xml_diff>
--- a/Definitions/b_Definitions_Tools.xlsx
+++ b/Definitions/b_Definitions_Tools.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="757" uniqueCount="657">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="759" uniqueCount="659">
   <si>
     <t>Topics</t>
   </si>
@@ -3311,6 +3311,12 @@
   </si>
   <si>
     <t>git push origin --all</t>
+  </si>
+  <si>
+    <t>revert local git commits</t>
+  </si>
+  <si>
+    <t>git reset --hard origin/&lt;master/branch name&gt;</t>
   </si>
 </sst>
 </file>
@@ -3527,7 +3533,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="82">
+  <cellXfs count="83">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -3670,6 +3676,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3677,12 +3685,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3717,7 +3725,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -4094,10 +4101,10 @@
       </c>
     </row>
     <row r="13" spans="1:3">
-      <c r="A13" s="64" t="s">
+      <c r="A13" s="66" t="s">
         <v>255</v>
       </c>
-      <c r="B13" s="65"/>
+      <c r="B13" s="67"/>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" s="1" t="s">
@@ -4143,10 +4150,10 @@
       </c>
     </row>
     <row r="23" spans="1:2">
-      <c r="A23" s="64" t="s">
+      <c r="A23" s="66" t="s">
         <v>331</v>
       </c>
-      <c r="B23" s="65"/>
+      <c r="B23" s="67"/>
     </row>
     <row r="24" spans="1:2">
       <c r="A24" s="1" t="s">
@@ -4159,10 +4166,10 @@
       </c>
     </row>
     <row r="27" spans="1:2">
-      <c r="A27" s="64" t="s">
+      <c r="A27" s="66" t="s">
         <v>616</v>
       </c>
-      <c r="B27" s="65"/>
+      <c r="B27" s="67"/>
     </row>
     <row r="28" spans="1:2">
       <c r="A28" s="1" t="s">
@@ -4228,10 +4235,10 @@
     </row>
     <row r="3" spans="1:2" s="17" customFormat="1"/>
     <row r="11" spans="1:2">
-      <c r="A11" s="64" t="s">
+      <c r="A11" s="66" t="s">
         <v>3</v>
       </c>
-      <c r="B11" s="65"/>
+      <c r="B11" s="67"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -4269,10 +4276,10 @@
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="64" t="s">
+      <c r="A2" s="66" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="65"/>
+      <c r="B2" s="67"/>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="58" t="s">
@@ -4339,7 +4346,7 @@
       </c>
     </row>
     <row r="11" spans="1:2">
-      <c r="A11" s="77" t="s">
+      <c r="A11" s="79" t="s">
         <v>635</v>
       </c>
       <c r="B11" s="59" t="s">
@@ -4347,7 +4354,7 @@
       </c>
     </row>
     <row r="12" spans="1:2">
-      <c r="A12" s="77"/>
+      <c r="A12" s="79"/>
       <c r="B12" s="59" t="s">
         <v>637</v>
       </c>
@@ -4417,10 +4424,10 @@
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="64" t="s">
+      <c r="A2" s="66" t="s">
         <v>254</v>
       </c>
-      <c r="B2" s="65"/>
+      <c r="B2" s="67"/>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="50" t="s">
@@ -4431,10 +4438,10 @@
       </c>
     </row>
     <row r="6" spans="1:2">
-      <c r="A6" s="64" t="s">
+      <c r="A6" s="66" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="65"/>
+      <c r="B6" s="67"/>
     </row>
     <row r="7" spans="1:2" ht="30">
       <c r="A7" s="49" t="s">
@@ -4453,7 +4460,7 @@
       </c>
     </row>
     <row r="9" spans="1:2">
-      <c r="A9" s="66" t="s">
+      <c r="A9" s="69" t="s">
         <v>265</v>
       </c>
       <c r="B9" s="22" t="s">
@@ -4461,13 +4468,13 @@
       </c>
     </row>
     <row r="10" spans="1:2">
-      <c r="A10" s="66"/>
+      <c r="A10" s="69"/>
       <c r="B10" s="22" t="s">
         <v>263</v>
       </c>
     </row>
     <row r="11" spans="1:2">
-      <c r="A11" s="66"/>
+      <c r="A11" s="69"/>
       <c r="B11" s="22" t="s">
         <v>261</v>
       </c>
@@ -4553,7 +4560,7 @@
       </c>
     </row>
     <row r="22" spans="1:2" ht="30">
-      <c r="A22" s="66" t="s">
+      <c r="A22" s="69" t="s">
         <v>542</v>
       </c>
       <c r="B22" s="48" t="s">
@@ -4561,13 +4568,13 @@
       </c>
     </row>
     <row r="23" spans="1:2" ht="60">
-      <c r="A23" s="66"/>
+      <c r="A23" s="69"/>
       <c r="B23" s="48" t="s">
         <v>544</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="45">
-      <c r="A24" s="70" t="s">
+      <c r="A24" s="72" t="s">
         <v>545</v>
       </c>
       <c r="B24" s="48" t="s">
@@ -4575,19 +4582,19 @@
       </c>
     </row>
     <row r="25" spans="1:2" ht="90">
-      <c r="A25" s="70"/>
+      <c r="A25" s="72"/>
       <c r="B25" s="48" t="s">
         <v>547</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="30">
-      <c r="A26" s="70"/>
+      <c r="A26" s="72"/>
       <c r="B26" s="48" t="s">
         <v>548</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="60">
-      <c r="A27" s="66" t="s">
+      <c r="A27" s="69" t="s">
         <v>549</v>
       </c>
       <c r="B27" s="48" t="s">
@@ -4595,19 +4602,19 @@
       </c>
     </row>
     <row r="28" spans="1:2" ht="45">
-      <c r="A28" s="66"/>
+      <c r="A28" s="69"/>
       <c r="B28" s="48" t="s">
         <v>552</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="45">
-      <c r="A29" s="66"/>
+      <c r="A29" s="69"/>
       <c r="B29" s="48" t="s">
         <v>551</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="60">
-      <c r="A30" s="79" t="s">
+      <c r="A30" s="81" t="s">
         <v>553</v>
       </c>
       <c r="B30" s="48" t="s">
@@ -4615,25 +4622,25 @@
       </c>
     </row>
     <row r="31" spans="1:2" ht="180">
-      <c r="A31" s="79"/>
+      <c r="A31" s="81"/>
       <c r="B31" s="48" t="s">
         <v>554</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="60">
-      <c r="A32" s="79"/>
+      <c r="A32" s="81"/>
       <c r="B32" s="48" t="s">
         <v>556</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="45">
-      <c r="A33" s="79"/>
+      <c r="A33" s="81"/>
       <c r="B33" s="48" t="s">
         <v>557</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="45">
-      <c r="A34" s="79" t="s">
+      <c r="A34" s="81" t="s">
         <v>558</v>
       </c>
       <c r="B34" s="48" t="s">
@@ -4641,19 +4648,19 @@
       </c>
     </row>
     <row r="35" spans="1:2" ht="105">
-      <c r="A35" s="79"/>
+      <c r="A35" s="81"/>
       <c r="B35" s="48" t="s">
         <v>560</v>
       </c>
     </row>
     <row r="36" spans="1:2">
-      <c r="A36" s="79"/>
+      <c r="A36" s="81"/>
       <c r="B36" s="48" t="s">
         <v>561</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="75">
-      <c r="A37" s="79" t="s">
+      <c r="A37" s="81" t="s">
         <v>562</v>
       </c>
       <c r="B37" s="48" t="s">
@@ -4661,25 +4668,25 @@
       </c>
     </row>
     <row r="38" spans="1:2" ht="120">
-      <c r="A38" s="79"/>
+      <c r="A38" s="81"/>
       <c r="B38" s="48" t="s">
         <v>564</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="45">
-      <c r="A39" s="79"/>
+      <c r="A39" s="81"/>
       <c r="B39" s="48" t="s">
         <v>565</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="45">
-      <c r="A40" s="79"/>
+      <c r="A40" s="81"/>
       <c r="B40" s="48" t="s">
         <v>566</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="60">
-      <c r="A41" s="79" t="s">
+      <c r="A41" s="81" t="s">
         <v>567</v>
       </c>
       <c r="B41" s="48" t="s">
@@ -4687,25 +4694,25 @@
       </c>
     </row>
     <row r="42" spans="1:2" ht="105">
-      <c r="A42" s="79"/>
+      <c r="A42" s="81"/>
       <c r="B42" s="48" t="s">
         <v>569</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="45">
-      <c r="A43" s="79"/>
+      <c r="A43" s="81"/>
       <c r="B43" s="48" t="s">
         <v>570</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="135">
-      <c r="A44" s="79"/>
+      <c r="A44" s="81"/>
       <c r="B44" s="48" t="s">
         <v>571</v>
       </c>
     </row>
     <row r="45" spans="1:2">
-      <c r="A45" s="79"/>
+      <c r="A45" s="81"/>
       <c r="B45" s="48" t="s">
         <v>572</v>
       </c>
@@ -4727,7 +4734,7 @@
       </c>
     </row>
     <row r="48" spans="1:2" ht="45">
-      <c r="A48" s="66" t="s">
+      <c r="A48" s="69" t="s">
         <v>576</v>
       </c>
       <c r="B48" s="49" t="s">
@@ -4735,13 +4742,13 @@
       </c>
     </row>
     <row r="49" spans="1:2">
-      <c r="A49" s="66"/>
+      <c r="A49" s="69"/>
       <c r="B49" s="49" t="s">
         <v>577</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="45">
-      <c r="A50" s="66" t="s">
+      <c r="A50" s="69" t="s">
         <v>578</v>
       </c>
       <c r="B50" s="49" t="s">
@@ -4749,19 +4756,19 @@
       </c>
     </row>
     <row r="51" spans="1:2" ht="135">
-      <c r="A51" s="66"/>
+      <c r="A51" s="69"/>
       <c r="B51" s="49" t="s">
         <v>581</v>
       </c>
     </row>
     <row r="52" spans="1:2">
-      <c r="A52" s="66"/>
+      <c r="A52" s="69"/>
       <c r="B52" s="49" t="s">
         <v>580</v>
       </c>
     </row>
     <row r="53" spans="1:2" ht="30">
-      <c r="A53" s="66" t="s">
+      <c r="A53" s="69" t="s">
         <v>584</v>
       </c>
       <c r="B53" s="49" t="s">
@@ -4769,7 +4776,7 @@
       </c>
     </row>
     <row r="54" spans="1:2" ht="60">
-      <c r="A54" s="66"/>
+      <c r="A54" s="69"/>
       <c r="B54" s="49" t="s">
         <v>587</v>
       </c>
@@ -4791,7 +4798,7 @@
       </c>
     </row>
     <row r="57" spans="1:2" ht="45">
-      <c r="A57" s="66" t="s">
+      <c r="A57" s="69" t="s">
         <v>590</v>
       </c>
       <c r="B57" s="49" t="s">
@@ -4799,7 +4806,7 @@
       </c>
     </row>
     <row r="58" spans="1:2">
-      <c r="A58" s="66"/>
+      <c r="A58" s="69"/>
       <c r="B58" s="49" t="s">
         <v>592</v>
       </c>
@@ -4920,10 +4927,10 @@
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="64" t="s">
+      <c r="A2" s="66" t="s">
         <v>254</v>
       </c>
-      <c r="B2" s="65"/>
+      <c r="B2" s="67"/>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="50" t="s">
@@ -4934,13 +4941,13 @@
       </c>
     </row>
     <row r="6" spans="1:2">
-      <c r="A6" s="64" t="s">
+      <c r="A6" s="66" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="65"/>
+      <c r="B6" s="67"/>
     </row>
     <row r="7" spans="1:2" ht="30">
-      <c r="A7" s="66" t="s">
+      <c r="A7" s="69" t="s">
         <v>224</v>
       </c>
       <c r="B7" s="22" t="s">
@@ -4948,7 +4955,7 @@
       </c>
     </row>
     <row r="8" spans="1:2" ht="30">
-      <c r="A8" s="66"/>
+      <c r="A8" s="69"/>
       <c r="B8" s="22" t="s">
         <v>274</v>
       </c>
@@ -4986,7 +4993,7 @@
       </c>
     </row>
     <row r="13" spans="1:2" ht="45">
-      <c r="A13" s="66" t="s">
+      <c r="A13" s="69" t="s">
         <v>506</v>
       </c>
       <c r="B13" s="40" t="s">
@@ -4994,7 +5001,7 @@
       </c>
     </row>
     <row r="14" spans="1:2" ht="45">
-      <c r="A14" s="73"/>
+      <c r="A14" s="75"/>
       <c r="B14" s="44" t="s">
         <v>505</v>
       </c>
@@ -5040,7 +5047,7 @@
       </c>
     </row>
     <row r="20" spans="1:2" ht="75">
-      <c r="A20" s="73" t="s">
+      <c r="A20" s="75" t="s">
         <v>517</v>
       </c>
       <c r="B20" s="48" t="s">
@@ -5048,13 +5055,13 @@
       </c>
     </row>
     <row r="21" spans="1:2" ht="75">
-      <c r="A21" s="73"/>
+      <c r="A21" s="75"/>
       <c r="B21" s="48" t="s">
         <v>519</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="30">
-      <c r="A22" s="80" t="s">
+      <c r="A22" s="82" t="s">
         <v>300</v>
       </c>
       <c r="B22" s="48" t="s">
@@ -5062,13 +5069,13 @@
       </c>
     </row>
     <row r="23" spans="1:2" ht="150">
-      <c r="A23" s="80"/>
+      <c r="A23" s="82"/>
       <c r="B23" s="48" t="s">
         <v>521</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="45">
-      <c r="A24" s="80" t="s">
+      <c r="A24" s="82" t="s">
         <v>454</v>
       </c>
       <c r="B24" s="48" t="s">
@@ -5076,13 +5083,13 @@
       </c>
     </row>
     <row r="25" spans="1:2" ht="150">
-      <c r="A25" s="80"/>
+      <c r="A25" s="82"/>
       <c r="B25" s="48" t="s">
         <v>523</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="60">
-      <c r="A26" s="73" t="s">
+      <c r="A26" s="75" t="s">
         <v>524</v>
       </c>
       <c r="B26" s="48" t="s">
@@ -5090,25 +5097,25 @@
       </c>
     </row>
     <row r="27" spans="1:2" ht="30">
-      <c r="A27" s="73"/>
+      <c r="A27" s="75"/>
       <c r="B27" s="48" t="s">
         <v>526</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="30">
-      <c r="A28" s="73"/>
+      <c r="A28" s="75"/>
       <c r="B28" s="48" t="s">
         <v>527</v>
       </c>
     </row>
     <row r="29" spans="1:2">
-      <c r="A29" s="73"/>
+      <c r="A29" s="75"/>
       <c r="B29" s="48" t="s">
         <v>528</v>
       </c>
     </row>
     <row r="30" spans="1:2">
-      <c r="A30" s="73" t="s">
+      <c r="A30" s="75" t="s">
         <v>531</v>
       </c>
       <c r="B30" s="48" t="s">
@@ -5116,7 +5123,7 @@
       </c>
     </row>
     <row r="31" spans="1:2" ht="30">
-      <c r="A31" s="73"/>
+      <c r="A31" s="75"/>
       <c r="B31" s="48" t="s">
         <v>530</v>
       </c>
@@ -5165,16 +5172,16 @@
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="64" t="s">
+      <c r="A2" s="66" t="s">
         <v>254</v>
       </c>
-      <c r="B2" s="65"/>
+      <c r="B2" s="67"/>
     </row>
     <row r="6" spans="1:2">
-      <c r="A6" s="64" t="s">
+      <c r="A6" s="66" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="65"/>
+      <c r="B6" s="67"/>
     </row>
     <row r="7" spans="1:2" ht="30">
       <c r="A7" s="22" t="s">
@@ -5230,10 +5237,10 @@
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="64" t="s">
+      <c r="A2" s="66" t="s">
         <v>254</v>
       </c>
-      <c r="B2" s="65"/>
+      <c r="B2" s="67"/>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="52" t="s">
@@ -5244,10 +5251,10 @@
       </c>
     </row>
     <row r="6" spans="1:2">
-      <c r="A6" s="64" t="s">
+      <c r="A6" s="66" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="65"/>
+      <c r="B6" s="67"/>
     </row>
     <row r="7" spans="1:2" ht="75">
       <c r="A7" s="53" t="s">
@@ -5311,16 +5318,16 @@
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="64" t="s">
+      <c r="A2" s="66" t="s">
         <v>254</v>
       </c>
-      <c r="B2" s="65"/>
+      <c r="B2" s="67"/>
     </row>
     <row r="6" spans="1:2">
-      <c r="A6" s="64" t="s">
+      <c r="A6" s="66" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="65"/>
+      <c r="B6" s="67"/>
     </row>
     <row r="7" spans="1:2" ht="45">
       <c r="A7" s="22" t="s">
@@ -5376,10 +5383,10 @@
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="64" t="s">
+      <c r="A2" s="66" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="65"/>
+      <c r="B2" s="67"/>
     </row>
     <row r="3" spans="1:2" ht="60">
       <c r="A3" s="30" t="s">
@@ -5690,10 +5697,10 @@
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="64" t="s">
+      <c r="A2" s="66" t="s">
         <v>228</v>
       </c>
-      <c r="B2" s="65"/>
+      <c r="B2" s="67"/>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="21" t="s">
@@ -5712,10 +5719,10 @@
       </c>
     </row>
     <row r="7" spans="1:2">
-      <c r="A7" s="64" t="s">
+      <c r="A7" s="66" t="s">
         <v>229</v>
       </c>
-      <c r="B7" s="65"/>
+      <c r="B7" s="67"/>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="6" t="s">
@@ -5732,10 +5739,10 @@
       <c r="A10" s="6"/>
     </row>
     <row r="11" spans="1:2">
-      <c r="A11" s="64" t="s">
+      <c r="A11" s="66" t="s">
         <v>103</v>
       </c>
-      <c r="B11" s="65"/>
+      <c r="B11" s="67"/>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="19" t="s">
@@ -5778,10 +5785,10 @@
       </c>
     </row>
     <row r="17" spans="1:2">
-      <c r="A17" s="64" t="s">
+      <c r="A17" s="66" t="s">
         <v>329</v>
       </c>
-      <c r="B17" s="65"/>
+      <c r="B17" s="67"/>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="31" t="s">
@@ -5792,10 +5799,10 @@
       </c>
     </row>
     <row r="20" spans="1:2">
-      <c r="A20" s="64" t="s">
+      <c r="A20" s="66" t="s">
         <v>436</v>
       </c>
-      <c r="B20" s="65"/>
+      <c r="B20" s="67"/>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" s="31" t="s">
@@ -5806,10 +5813,10 @@
       </c>
     </row>
     <row r="23" spans="1:2">
-      <c r="A23" s="64" t="s">
+      <c r="A23" s="66" t="s">
         <v>209</v>
       </c>
-      <c r="B23" s="65"/>
+      <c r="B23" s="67"/>
     </row>
     <row r="24" spans="1:2">
       <c r="A24" s="17" t="s">
@@ -5836,10 +5843,10 @@
       </c>
     </row>
     <row r="28" spans="1:2">
-      <c r="A28" s="64" t="s">
+      <c r="A28" s="66" t="s">
         <v>205</v>
       </c>
-      <c r="B28" s="65"/>
+      <c r="B28" s="67"/>
     </row>
     <row r="29" spans="1:2">
       <c r="A29" s="17" t="s">
@@ -5858,10 +5865,10 @@
       </c>
     </row>
     <row r="32" spans="1:2">
-      <c r="A32" s="64" t="s">
+      <c r="A32" s="66" t="s">
         <v>104</v>
       </c>
-      <c r="B32" s="65"/>
+      <c r="B32" s="67"/>
     </row>
     <row r="33" spans="1:2">
       <c r="A33" s="19" t="s">
@@ -5880,10 +5887,10 @@
       </c>
     </row>
     <row r="36" spans="1:2">
-      <c r="A36" s="64" t="s">
+      <c r="A36" s="66" t="s">
         <v>168</v>
       </c>
-      <c r="B36" s="65"/>
+      <c r="B36" s="67"/>
     </row>
     <row r="37" spans="1:2">
       <c r="A37" s="19" t="s">
@@ -5894,10 +5901,10 @@
       </c>
     </row>
     <row r="39" spans="1:2">
-      <c r="A39" s="64" t="s">
+      <c r="A39" s="66" t="s">
         <v>171</v>
       </c>
-      <c r="B39" s="65"/>
+      <c r="B39" s="67"/>
     </row>
     <row r="40" spans="1:2">
       <c r="A40" t="s">
@@ -5914,16 +5921,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="A39:B39"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="A11:B11"/>
     <mergeCell ref="A17:B17"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="A39:B39"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B1" location="Materials!A2" display="Up"/>
@@ -5971,10 +5978,10 @@
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="64" t="s">
+      <c r="A2" s="66" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="65"/>
+      <c r="B2" s="67"/>
     </row>
     <row r="3" spans="1:2" ht="45">
       <c r="A3" s="30" t="s">
@@ -6141,11 +6148,11 @@
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A14" sqref="A14"/>
+      <selection pane="bottomLeft" activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6163,10 +6170,10 @@
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="64" t="s">
+      <c r="A2" s="66" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="65"/>
+      <c r="B2" s="67"/>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="56" t="s">
@@ -6233,7 +6240,7 @@
       </c>
     </row>
     <row r="11" spans="1:2">
-      <c r="A11" s="77" t="s">
+      <c r="A11" s="79" t="s">
         <v>650</v>
       </c>
       <c r="B11" s="61" t="s">
@@ -6241,17 +6248,25 @@
       </c>
     </row>
     <row r="12" spans="1:2">
-      <c r="A12" s="77"/>
+      <c r="A12" s="79"/>
       <c r="B12" s="61" t="s">
         <v>652</v>
       </c>
     </row>
     <row r="13" spans="1:2">
-      <c r="A13" s="81" t="s">
+      <c r="A13" s="65" t="s">
         <v>655</v>
       </c>
       <c r="B13" s="63" t="s">
         <v>656</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" s="65" t="s">
+        <v>657</v>
+      </c>
+      <c r="B14" s="64" t="s">
+        <v>658</v>
       </c>
     </row>
   </sheetData>
@@ -6291,10 +6306,10 @@
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="64" t="s">
+      <c r="A2" s="66" t="s">
         <v>254</v>
       </c>
-      <c r="B2" s="65"/>
+      <c r="B2" s="67"/>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="24" t="s">
@@ -6305,10 +6320,10 @@
       </c>
     </row>
     <row r="10" spans="1:2">
-      <c r="A10" s="64" t="s">
+      <c r="A10" s="66" t="s">
         <v>3</v>
       </c>
-      <c r="B10" s="65"/>
+      <c r="B10" s="67"/>
     </row>
     <row r="11" spans="1:2" ht="45">
       <c r="A11" s="6" t="s">
@@ -6413,7 +6428,7 @@
       </c>
     </row>
     <row r="24" spans="1:2">
-      <c r="A24" s="70" t="s">
+      <c r="A24" s="72" t="s">
         <v>29</v>
       </c>
       <c r="B24" s="6" t="s">
@@ -6421,7 +6436,7 @@
       </c>
     </row>
     <row r="25" spans="1:2">
-      <c r="A25" s="70"/>
+      <c r="A25" s="72"/>
       <c r="B25" s="6" t="s">
         <v>31</v>
       </c>
@@ -6467,7 +6482,7 @@
       </c>
     </row>
     <row r="31" spans="1:2" ht="45">
-      <c r="A31" s="69" t="s">
+      <c r="A31" s="71" t="s">
         <v>42</v>
       </c>
       <c r="B31" s="51" t="s">
@@ -6475,7 +6490,7 @@
       </c>
     </row>
     <row r="32" spans="1:2" ht="120">
-      <c r="A32" s="69"/>
+      <c r="A32" s="71"/>
       <c r="B32" s="51" t="s">
         <v>43</v>
       </c>
@@ -6553,7 +6568,7 @@
       </c>
     </row>
     <row r="42" spans="1:2" ht="75">
-      <c r="A42" s="67" t="s">
+      <c r="A42" s="70" t="s">
         <v>64</v>
       </c>
       <c r="B42" s="6" t="s">
@@ -6561,7 +6576,7 @@
       </c>
     </row>
     <row r="43" spans="1:2">
-      <c r="A43" s="67"/>
+      <c r="A43" s="70"/>
       <c r="B43" s="6" t="s">
         <v>66</v>
       </c>
@@ -6599,7 +6614,7 @@
       </c>
     </row>
     <row r="48" spans="1:2" ht="45">
-      <c r="A48" s="67" t="s">
+      <c r="A48" s="70" t="s">
         <v>77</v>
       </c>
       <c r="B48" s="6" t="s">
@@ -6607,19 +6622,19 @@
       </c>
     </row>
     <row r="49" spans="1:2" ht="45">
-      <c r="A49" s="67"/>
+      <c r="A49" s="70"/>
       <c r="B49" s="6" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="45">
-      <c r="A50" s="67"/>
+      <c r="A50" s="70"/>
       <c r="B50" s="6" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="51" spans="1:2" ht="45">
-      <c r="A51" s="67" t="s">
+      <c r="A51" s="70" t="s">
         <v>78</v>
       </c>
       <c r="B51" s="6" t="s">
@@ -6627,13 +6642,13 @@
       </c>
     </row>
     <row r="52" spans="1:2" ht="60">
-      <c r="A52" s="67"/>
+      <c r="A52" s="70"/>
       <c r="B52" s="6" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="53" spans="1:2" ht="45">
-      <c r="A53" s="67"/>
+      <c r="A53" s="70"/>
       <c r="B53" s="6" t="s">
         <v>81</v>
       </c>
@@ -6743,7 +6758,7 @@
       </c>
     </row>
     <row r="68" spans="1:2">
-      <c r="A68" s="66" t="s">
+      <c r="A68" s="69" t="s">
         <v>251</v>
       </c>
       <c r="B68" s="22" t="s">
@@ -6751,7 +6766,7 @@
       </c>
     </row>
     <row r="69" spans="1:2">
-      <c r="A69" s="66"/>
+      <c r="A69" s="69"/>
       <c r="B69" s="22" t="s">
         <v>249</v>
       </c>
@@ -6773,7 +6788,7 @@
       </c>
     </row>
     <row r="72" spans="1:2">
-      <c r="A72" s="66" t="s">
+      <c r="A72" s="69" t="s">
         <v>247</v>
       </c>
       <c r="B72" s="22" t="s">
@@ -6781,7 +6796,7 @@
       </c>
     </row>
     <row r="73" spans="1:2">
-      <c r="A73" s="66"/>
+      <c r="A73" s="69"/>
       <c r="B73" s="22" t="s">
         <v>244</v>
       </c>
@@ -6961,7 +6976,7 @@
       </c>
     </row>
     <row r="96" spans="1:2">
-      <c r="A96" s="66" t="s">
+      <c r="A96" s="69" t="s">
         <v>305</v>
       </c>
       <c r="B96" s="28" t="s">
@@ -6969,13 +6984,13 @@
       </c>
     </row>
     <row r="97" spans="1:2">
-      <c r="A97" s="66"/>
+      <c r="A97" s="69"/>
       <c r="B97" s="28" t="s">
         <v>309</v>
       </c>
     </row>
     <row r="98" spans="1:2" ht="45">
-      <c r="A98" s="66" t="s">
+      <c r="A98" s="69" t="s">
         <v>313</v>
       </c>
       <c r="B98" s="28" t="s">
@@ -6983,7 +6998,7 @@
       </c>
     </row>
     <row r="99" spans="1:2">
-      <c r="A99" s="66"/>
+      <c r="A99" s="69"/>
       <c r="B99" s="28" t="s">
         <v>315</v>
       </c>
@@ -7003,7 +7018,7 @@
       </c>
     </row>
     <row r="102" spans="1:2" ht="60">
-      <c r="A102" s="66" t="s">
+      <c r="A102" s="69" t="s">
         <v>319</v>
       </c>
       <c r="B102" s="28" t="s">
@@ -7011,13 +7026,13 @@
       </c>
     </row>
     <row r="103" spans="1:2">
-      <c r="A103" s="66"/>
+      <c r="A103" s="69"/>
       <c r="B103" s="28" t="s">
         <v>321</v>
       </c>
     </row>
     <row r="104" spans="1:2" ht="90">
-      <c r="A104" s="66" t="s">
+      <c r="A104" s="69" t="s">
         <v>322</v>
       </c>
       <c r="B104" s="28" t="s">
@@ -7025,13 +7040,13 @@
       </c>
     </row>
     <row r="105" spans="1:2">
-      <c r="A105" s="66"/>
+      <c r="A105" s="69"/>
       <c r="B105" s="28" t="s">
         <v>324</v>
       </c>
     </row>
     <row r="106" spans="1:2" ht="30">
-      <c r="A106" s="66" t="s">
+      <c r="A106" s="69" t="s">
         <v>325</v>
       </c>
       <c r="B106" s="29" t="s">
@@ -7039,13 +7054,13 @@
       </c>
     </row>
     <row r="107" spans="1:2">
-      <c r="A107" s="66"/>
+      <c r="A107" s="69"/>
       <c r="B107" s="29" t="s">
         <v>327</v>
       </c>
     </row>
     <row r="108" spans="1:2" ht="45">
-      <c r="A108" s="66" t="s">
+      <c r="A108" s="69" t="s">
         <v>454</v>
       </c>
       <c r="B108" s="40" t="s">
@@ -7053,13 +7068,13 @@
       </c>
     </row>
     <row r="109" spans="1:2" ht="75">
-      <c r="A109" s="66"/>
+      <c r="A109" s="69"/>
       <c r="B109" s="40" t="s">
         <v>455</v>
       </c>
     </row>
     <row r="110" spans="1:2" ht="45">
-      <c r="A110" s="66" t="s">
+      <c r="A110" s="69" t="s">
         <v>457</v>
       </c>
       <c r="B110" s="40" t="s">
@@ -7067,13 +7082,13 @@
       </c>
     </row>
     <row r="111" spans="1:2" ht="75">
-      <c r="A111" s="66"/>
+      <c r="A111" s="69"/>
       <c r="B111" s="40" t="s">
         <v>459</v>
       </c>
     </row>
     <row r="112" spans="1:2">
-      <c r="A112" s="66" t="s">
+      <c r="A112" s="69" t="s">
         <v>460</v>
       </c>
       <c r="B112" s="40" t="s">
@@ -7081,13 +7096,13 @@
       </c>
     </row>
     <row r="113" spans="1:2" ht="60">
-      <c r="A113" s="66"/>
+      <c r="A113" s="69"/>
       <c r="B113" s="40" t="s">
         <v>462</v>
       </c>
     </row>
     <row r="114" spans="1:2">
-      <c r="A114" s="66" t="s">
+      <c r="A114" s="69" t="s">
         <v>463</v>
       </c>
       <c r="B114" s="40" t="s">
@@ -7095,13 +7110,13 @@
       </c>
     </row>
     <row r="115" spans="1:2" ht="75">
-      <c r="A115" s="66"/>
+      <c r="A115" s="69"/>
       <c r="B115" s="40" t="s">
         <v>465</v>
       </c>
     </row>
     <row r="116" spans="1:2" ht="60">
-      <c r="A116" s="66" t="s">
+      <c r="A116" s="69" t="s">
         <v>466</v>
       </c>
       <c r="B116" s="40" t="s">
@@ -7109,7 +7124,7 @@
       </c>
     </row>
     <row r="117" spans="1:2" ht="60">
-      <c r="A117" s="66"/>
+      <c r="A117" s="69"/>
       <c r="B117" s="40" t="s">
         <v>468</v>
       </c>
@@ -7131,7 +7146,7 @@
       </c>
     </row>
     <row r="120" spans="1:2" ht="60">
-      <c r="A120" s="66" t="s">
+      <c r="A120" s="69" t="s">
         <v>473</v>
       </c>
       <c r="B120" s="40" t="s">
@@ -7139,19 +7154,19 @@
       </c>
     </row>
     <row r="121" spans="1:2" ht="60">
-      <c r="A121" s="66"/>
+      <c r="A121" s="69"/>
       <c r="B121" s="40" t="s">
         <v>475</v>
       </c>
     </row>
     <row r="122" spans="1:2">
-      <c r="A122" s="66"/>
+      <c r="A122" s="69"/>
       <c r="B122" s="40" t="s">
         <v>476</v>
       </c>
     </row>
     <row r="123" spans="1:2" ht="75">
-      <c r="A123" s="66" t="s">
+      <c r="A123" s="69" t="s">
         <v>477</v>
       </c>
       <c r="B123" s="40" t="s">
@@ -7159,13 +7174,32 @@
       </c>
     </row>
     <row r="124" spans="1:2" ht="135">
-      <c r="A124" s="66"/>
+      <c r="A124" s="69"/>
       <c r="B124" s="40" t="s">
         <v>479</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="26">
+    <mergeCell ref="A120:A122"/>
+    <mergeCell ref="A123:A124"/>
+    <mergeCell ref="A108:A109"/>
+    <mergeCell ref="A110:A111"/>
+    <mergeCell ref="A112:A113"/>
+    <mergeCell ref="A114:A115"/>
+    <mergeCell ref="A116:A117"/>
+    <mergeCell ref="A68:A69"/>
+    <mergeCell ref="A72:A73"/>
+    <mergeCell ref="A48:A50"/>
+    <mergeCell ref="A51:A53"/>
+    <mergeCell ref="A57:A60"/>
+    <mergeCell ref="A62:A63"/>
+    <mergeCell ref="A42:A43"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A31:A32"/>
+    <mergeCell ref="A22:A23"/>
+    <mergeCell ref="A24:A25"/>
     <mergeCell ref="A100:A101"/>
     <mergeCell ref="A102:A103"/>
     <mergeCell ref="A104:A105"/>
@@ -7173,25 +7207,6 @@
     <mergeCell ref="A85:A86"/>
     <mergeCell ref="A96:A97"/>
     <mergeCell ref="A98:A99"/>
-    <mergeCell ref="A42:A43"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A31:A32"/>
-    <mergeCell ref="A22:A23"/>
-    <mergeCell ref="A24:A25"/>
-    <mergeCell ref="A68:A69"/>
-    <mergeCell ref="A72:A73"/>
-    <mergeCell ref="A48:A50"/>
-    <mergeCell ref="A51:A53"/>
-    <mergeCell ref="A57:A60"/>
-    <mergeCell ref="A62:A63"/>
-    <mergeCell ref="A120:A122"/>
-    <mergeCell ref="A123:A124"/>
-    <mergeCell ref="A108:A109"/>
-    <mergeCell ref="A110:A111"/>
-    <mergeCell ref="A112:A113"/>
-    <mergeCell ref="A114:A115"/>
-    <mergeCell ref="A116:A117"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B1" location="JSON!A2" display="Up"/>
@@ -7231,16 +7246,16 @@
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="64" t="s">
+      <c r="A2" s="66" t="s">
         <v>254</v>
       </c>
-      <c r="B2" s="65"/>
+      <c r="B2" s="67"/>
     </row>
     <row r="5" spans="1:2">
-      <c r="A5" s="64" t="s">
+      <c r="A5" s="66" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="65"/>
+      <c r="B5" s="67"/>
     </row>
     <row r="6" spans="1:2" ht="45">
       <c r="A6" t="s">
@@ -7305,10 +7320,10 @@
     </row>
     <row r="3" spans="1:2" s="19" customFormat="1"/>
     <row r="9" spans="1:2">
-      <c r="A9" s="64" t="s">
+      <c r="A9" s="66" t="s">
         <v>3</v>
       </c>
-      <c r="B9" s="65"/>
+      <c r="B9" s="67"/>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
@@ -7363,19 +7378,19 @@
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="64" t="s">
+      <c r="A2" s="66" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="65"/>
+      <c r="B2" s="67"/>
     </row>
     <row r="9" spans="1:2">
-      <c r="A9" s="64" t="s">
+      <c r="A9" s="66" t="s">
         <v>3</v>
       </c>
-      <c r="B9" s="65"/>
+      <c r="B9" s="67"/>
     </row>
     <row r="10" spans="1:2" ht="75">
-      <c r="A10" s="72" t="s">
+      <c r="A10" s="74" t="s">
         <v>112</v>
       </c>
       <c r="B10" s="54" t="s">
@@ -7383,7 +7398,7 @@
       </c>
     </row>
     <row r="11" spans="1:2">
-      <c r="A11" s="66"/>
+      <c r="A11" s="69"/>
       <c r="B11" s="11" t="s">
         <v>114</v>
       </c>
@@ -7397,7 +7412,7 @@
       </c>
     </row>
     <row r="13" spans="1:2">
-      <c r="A13" s="66" t="s">
+      <c r="A13" s="69" t="s">
         <v>117</v>
       </c>
       <c r="B13" s="54" t="s">
@@ -7405,7 +7420,7 @@
       </c>
     </row>
     <row r="14" spans="1:2">
-      <c r="A14" s="66"/>
+      <c r="A14" s="69"/>
       <c r="B14" s="54" t="s">
         <v>119</v>
       </c>
@@ -7443,7 +7458,7 @@
       </c>
     </row>
     <row r="19" spans="1:2" ht="60">
-      <c r="A19" s="66" t="s">
+      <c r="A19" s="69" t="s">
         <v>128</v>
       </c>
       <c r="B19" s="54" t="s">
@@ -7451,13 +7466,13 @@
       </c>
     </row>
     <row r="20" spans="1:2">
-      <c r="A20" s="66"/>
+      <c r="A20" s="69"/>
       <c r="B20" s="54" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="21" spans="1:2">
-      <c r="A21" s="66" t="s">
+      <c r="A21" s="69" t="s">
         <v>131</v>
       </c>
       <c r="B21" s="54" t="s">
@@ -7465,16 +7480,16 @@
       </c>
     </row>
     <row r="22" spans="1:2">
-      <c r="A22" s="66"/>
+      <c r="A22" s="69"/>
       <c r="B22" s="54" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="23" spans="1:2">
-      <c r="A23" s="71" t="s">
+      <c r="A23" s="73" t="s">
         <v>134</v>
       </c>
-      <c r="B23" s="71"/>
+      <c r="B23" s="73"/>
     </row>
     <row r="24" spans="1:2" ht="60">
       <c r="A24" s="55" t="s">
@@ -7581,7 +7596,7 @@
       </c>
     </row>
     <row r="37" spans="1:2">
-      <c r="A37" s="66" t="s">
+      <c r="A37" s="69" t="s">
         <v>161</v>
       </c>
       <c r="B37" s="11" t="s">
@@ -7589,7 +7604,7 @@
       </c>
     </row>
     <row r="38" spans="1:2" ht="60">
-      <c r="A38" s="66"/>
+      <c r="A38" s="69"/>
       <c r="B38" s="54" t="s">
         <v>163</v>
       </c>
@@ -7662,16 +7677,16 @@
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="64" t="s">
+      <c r="A2" s="66" t="s">
         <v>254</v>
       </c>
-      <c r="B2" s="65"/>
+      <c r="B2" s="67"/>
     </row>
     <row r="6" spans="1:2">
-      <c r="A6" s="64" t="s">
+      <c r="A6" s="66" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="65"/>
+      <c r="B6" s="67"/>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="43" t="s">
@@ -7682,7 +7697,7 @@
       </c>
     </row>
     <row r="8" spans="1:2" ht="105">
-      <c r="A8" s="73" t="s">
+      <c r="A8" s="75" t="s">
         <v>487</v>
       </c>
       <c r="B8" s="42" t="s">
@@ -7690,7 +7705,7 @@
       </c>
     </row>
     <row r="9" spans="1:2" ht="105">
-      <c r="A9" s="73"/>
+      <c r="A9" s="75"/>
       <c r="B9" s="42" t="s">
         <v>489</v>
       </c>
@@ -7822,20 +7837,20 @@
       </c>
     </row>
     <row r="2" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A2" s="74" t="s">
+      <c r="A2" s="76" t="s">
         <v>172</v>
       </c>
-      <c r="B2" s="75"/>
+      <c r="B2" s="77"/>
     </row>
     <row r="8" spans="1:2" ht="15.75" thickBot="1"/>
     <row r="9" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A9" s="74" t="s">
+      <c r="A9" s="76" t="s">
         <v>3</v>
       </c>
-      <c r="B9" s="75"/>
+      <c r="B9" s="77"/>
     </row>
     <row r="10" spans="1:2">
-      <c r="A10" s="76" t="s">
+      <c r="A10" s="78" t="s">
         <v>185</v>
       </c>
       <c r="B10" t="s">
@@ -7843,13 +7858,13 @@
       </c>
     </row>
     <row r="11" spans="1:2">
-      <c r="A11" s="77"/>
+      <c r="A11" s="79"/>
       <c r="B11" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="12" spans="1:2">
-      <c r="A12" s="78" t="s">
+      <c r="A12" s="80" t="s">
         <v>182</v>
       </c>
       <c r="B12" t="s">
@@ -7857,13 +7872,13 @@
       </c>
     </row>
     <row r="13" spans="1:2" ht="45">
-      <c r="A13" s="78"/>
+      <c r="A13" s="80"/>
       <c r="B13" s="14" t="s">
         <v>180</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="60">
-      <c r="A14" s="78"/>
+      <c r="A14" s="80"/>
       <c r="B14" s="14" t="s">
         <v>179</v>
       </c>

</xml_diff>